<commit_message>
Final clustering for write-up
</commit_message>
<xml_diff>
--- a/clustering/Optimal Clusters.xlsx
+++ b/clustering/Optimal Clusters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sats\Desktop\3B\MSCI 446\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sats\Desktop\justgetstarted\clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="With Health Score" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Number of Clusters against Sum of Distances from Sample to Cluster Center</a:t>
+              <a:t>Number of Clusters against Sum of Distances from Samples to Cluster Center</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -675,143 +675,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Without Health Score'!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Clusters</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Without Health Score'!$A$2:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Without Health Score'!$A$2:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4773-463D-9964-70E7115B100A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Without Health Score'!$B$1</c:f>
@@ -893,46 +758,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>87249.867001899998</c:v>
+                  <c:v>23.752231405500002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59578.480472199997</c:v>
+                  <c:v>19.512200162199999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44944.1957731</c:v>
+                  <c:v>16.4007603166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37804.398361300002</c:v>
+                  <c:v>14.5465074082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30794.8295153</c:v>
+                  <c:v>13.3865741575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26707.139217200001</c:v>
+                  <c:v>12.5020182176</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22921.926653400002</c:v>
+                  <c:v>11.7120864315</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20426.8203101</c:v>
+                  <c:v>11.1225947143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18537.974248800001</c:v>
+                  <c:v>10.473917637</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16605.2168762</c:v>
+                  <c:v>10.015981801000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14948.178927200001</c:v>
+                  <c:v>9.6170648940200003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14036.685256299999</c:v>
+                  <c:v>9.2533050724599999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12737.524740999999</c:v>
+                  <c:v>8.8949920363300006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11912.1906473</c:v>
+                  <c:v>8.5354125581000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2383,13 +2248,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2716,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2855,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2742,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>87249.867001899998</v>
+        <v>23.752231405500002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2885,7 +2750,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>59578.480472199997</v>
+        <v>19.512200162199999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2893,7 +2758,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>44944.1957731</v>
+        <v>16.4007603166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,7 +2766,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>37804.398361300002</v>
+        <v>14.5465074082</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2909,7 +2774,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>30794.8295153</v>
+        <v>13.3865741575</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2917,7 +2782,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>26707.139217200001</v>
+        <v>12.5020182176</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2925,7 +2790,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>22921.926653400002</v>
+        <v>11.7120864315</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,7 +2798,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>20426.8203101</v>
+        <v>11.1225947143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2941,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>18537.974248800001</v>
+        <v>10.473917637</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2949,7 +2814,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>16605.2168762</v>
+        <v>10.015981801000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2957,7 +2822,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>14948.178927200001</v>
+        <v>9.6170648940200003</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,7 +2830,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>14036.685256299999</v>
+        <v>9.2533050724599999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,7 +2838,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>12737.524740999999</v>
+        <v>8.8949920363300006</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2981,7 +2846,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>11912.1906473</v>
+        <v>8.5354125581000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>